<commit_message>
change everything to the things devora wanted: adding/removing fields removing hall and ride exports adding family invitation
</commit_message>
<xml_diff>
--- a/all_info.xlsx
+++ b/all_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>invitation #</t>
   </si>
@@ -55,6 +55,45 @@
     <t>url</t>
   </si>
   <si>
+    <t>60107</t>
+  </si>
+  <si>
+    <t>regular invitation</t>
+  </si>
+  <si>
+    <t>testing person 1</t>
+  </si>
+  <si>
+    <t>טסטינג פרסון 1</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Groom</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>1@1.com</t>
+  </si>
+  <si>
+    <t>avichaidevora.com/invitation/60107</t>
+  </si>
+  <si>
+    <t>testing person 2</t>
+  </si>
+  <si>
+    <t>טסטינג פרסון 2</t>
+  </si>
+  <si>
+    <t>2@2.com</t>
+  </si>
+  <si>
     <t>42652</t>
   </si>
   <si>
@@ -67,10 +106,10 @@
     <t>משפחת מוסקוביץ</t>
   </si>
   <si>
-    <t>Maybe</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Allergies</t>
   </si>
   <si>
     <t>Bride</t>
@@ -83,39 +122,6 @@
   </si>
   <si>
     <t>avichaidevora.com/invitation/42652</t>
-  </si>
-  <si>
-    <t>60107</t>
-  </si>
-  <si>
-    <t>regular invitation</t>
-  </si>
-  <si>
-    <t>testing person 1</t>
-  </si>
-  <si>
-    <t>טסטינג פרסון 1</t>
-  </si>
-  <si>
-    <t>Groom</t>
-  </si>
-  <si>
-    <t>Work</t>
-  </si>
-  <si>
-    <t>1@1.com</t>
-  </si>
-  <si>
-    <t>avichaidevora.com/invitation/60107</t>
-  </si>
-  <si>
-    <t>testing person 2</t>
-  </si>
-  <si>
-    <t>טסטינג פרסון 2</t>
-  </si>
-  <si>
-    <t>2@2.com</t>
   </si>
   <si>
     <t>20349</t>
@@ -579,7 +585,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -603,16 +609,16 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>17</v>
@@ -628,69 +634,71 @@
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="J4" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>17</v>
@@ -706,30 +714,30 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>17</v>
@@ -745,14 +753,14 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small fixes and added re-close action failed attempt at intermediary admin page changed family_rsvp to person rsvp
</commit_message>
<xml_diff>
--- a/all_info.xlsx
+++ b/all_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>invitation #</t>
   </si>
@@ -70,7 +70,7 @@
     <t>Maybe</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>2015-04-19 17:07</t>
   </si>
   <si>
     <t>Groom</t>
@@ -109,7 +109,7 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Allergies</t>
+    <t>2015-04-19 21:41</t>
   </si>
   <si>
     <t>Bride</t>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>חבר מהצבא</t>
+  </si>
+  <si>
+    <t>2015-04-19 19:01</t>
+  </si>
+  <si>
+    <t>Vegan</t>
   </si>
   <si>
     <t>Army</t>
@@ -666,14 +672,12 @@
         <v>5</v>
       </c>
       <c r="G4" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
         <v>32</v>
       </c>
@@ -701,29 +705,31 @@
         <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="J5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>34</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -734,10 +740,10 @@
         <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>17</v>
@@ -746,21 +752,21 @@
         <v>1</v>
       </c>
       <c r="G6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor text fixes and used choices appropriately added gluten free
</commit_message>
<xml_diff>
--- a/all_info.xlsx
+++ b/all_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>invitation #</t>
   </si>
@@ -67,91 +67,118 @@
     <t>טסטינג פרסון 1</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>2015-04-23 10:11</t>
+  </si>
+  <si>
+    <t>Vegan</t>
+  </si>
+  <si>
+    <t>Groom</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>1@1.com</t>
+  </si>
+  <si>
+    <t>avichaidevora.com/invitation/60107</t>
+  </si>
+  <si>
+    <t>testing person 2</t>
+  </si>
+  <si>
+    <t>טסטינג פרסון 2</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>GlutenFree</t>
+  </si>
+  <si>
+    <t>2@2.com</t>
+  </si>
+  <si>
+    <t>42652</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>the Moskovitzes</t>
+  </si>
+  <si>
+    <t>משפחת מוסקוביץ</t>
+  </si>
+  <si>
+    <t>2015-04-23 10:08</t>
+  </si>
+  <si>
+    <t>Bride</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>reyley1014@gmail.com</t>
+  </si>
+  <si>
+    <t>avichaidevora.com/invitation/42652</t>
+  </si>
+  <si>
+    <t>20349</t>
+  </si>
+  <si>
+    <t>with guest</t>
+  </si>
+  <si>
+    <t>army friend</t>
+  </si>
+  <si>
+    <t>חבר מהצבא</t>
+  </si>
+  <si>
+    <t>2015-04-23 10:19</t>
+  </si>
+  <si>
+    <t>Army</t>
+  </si>
+  <si>
+    <t>avichaidevora.com/invitation/20349</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>אורח/ת</t>
+  </si>
+  <si>
     <t>Maybe</t>
   </si>
   <si>
-    <t>2015-04-19 17:07</t>
-  </si>
-  <si>
-    <t>Groom</t>
-  </si>
-  <si>
-    <t>Work</t>
-  </si>
-  <si>
-    <t>1@1.com</t>
-  </si>
-  <si>
-    <t>avichaidevora.com/invitation/60107</t>
-  </si>
-  <si>
-    <t>testing person 2</t>
-  </si>
-  <si>
-    <t>טסטינג פרסון 2</t>
-  </si>
-  <si>
-    <t>2@2.com</t>
-  </si>
-  <si>
-    <t>42652</t>
-  </si>
-  <si>
-    <t>family</t>
-  </si>
-  <si>
-    <t>the Moskovitzes</t>
-  </si>
-  <si>
-    <t>משפחת מוסקוביץ</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>2015-04-19 21:41</t>
-  </si>
-  <si>
-    <t>Bride</t>
-  </si>
-  <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>reyley1014@gmail.com</t>
-  </si>
-  <si>
-    <t>avichaidevora.com/invitation/42652</t>
-  </si>
-  <si>
-    <t>20349</t>
-  </si>
-  <si>
-    <t>with guest</t>
-  </si>
-  <si>
-    <t>army friend</t>
-  </si>
-  <si>
-    <t>חבר מהצבא</t>
-  </si>
-  <si>
-    <t>2015-04-19 19:01</t>
-  </si>
-  <si>
-    <t>Vegan</t>
-  </si>
-  <si>
-    <t>Army</t>
-  </si>
-  <si>
-    <t>avichaidevora.com/invitation/20349</t>
-  </si>
-  <si>
-    <t>Guest</t>
-  </si>
-  <si>
-    <t>אורח/ת</t>
+    <t>88850</t>
+  </si>
+  <si>
+    <t>sththrtger</t>
+  </si>
+  <si>
+    <t>srhsth</t>
+  </si>
+  <si>
+    <t>httshtrh</t>
+  </si>
+  <si>
+    <t>2015-04-21 16:57</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>avichaidevora.com/invitation/88850</t>
   </si>
 </sst>
 </file>
@@ -508,7 +535,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -517,11 +544,11 @@
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
@@ -599,18 +626,20 @@
       <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="J2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -621,52 +650,54 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F4" s="2">
         <v>5</v>
@@ -675,78 +706,78 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="M5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -755,18 +786,55 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add diet families to statistics page and changes action so it sets the whole invitation back to default
</commit_message>
<xml_diff>
--- a/all_info.xlsx
+++ b/all_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>invitation #</t>
   </si>
@@ -157,19 +157,22 @@
     <t>אורח/ת</t>
   </si>
   <si>
+    <t>Vegetarian</t>
+  </si>
+  <si>
+    <t>88850</t>
+  </si>
+  <si>
+    <t>sththrtger</t>
+  </si>
+  <si>
+    <t>srhsth</t>
+  </si>
+  <si>
+    <t>httshtrh</t>
+  </si>
+  <si>
     <t>Maybe</t>
-  </si>
-  <si>
-    <t>88850</t>
-  </si>
-  <si>
-    <t>sththrtger</t>
-  </si>
-  <si>
-    <t>srhsth</t>
-  </si>
-  <si>
-    <t>httshtrh</t>
   </si>
   <si>
     <t>2015-04-21 16:57</t>
@@ -777,7 +780,7 @@
         <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -788,7 +791,9 @@
       <c r="H6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="J6" s="2" t="s">
         <v>20</v>
       </c>
@@ -814,7 +819,7 @@
         <v>51</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -823,18 +828,18 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed email name for a couple and added language to the export
</commit_message>
<xml_diff>
--- a/all_info.xlsx
+++ b/all_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
   <si>
     <t>invitation #</t>
   </si>
@@ -22,10 +22,13 @@
     <t>invitation name</t>
   </si>
   <si>
-    <t>guest english name</t>
-  </si>
-  <si>
-    <t>guest hebrew name</t>
+    <t>English name</t>
+  </si>
+  <si>
+    <t>Hebrew name</t>
+  </si>
+  <si>
+    <t>Language</t>
   </si>
   <si>
     <t>RSVP</t>
@@ -55,6 +58,69 @@
     <t>url</t>
   </si>
   <si>
+    <t>42652</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>the Moskovitzes</t>
+  </si>
+  <si>
+    <t>משפחת מוסקוביץ</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>2015-04-26 18:24</t>
+  </si>
+  <si>
+    <t>Bride</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>reyley1014@gmail.com</t>
+  </si>
+  <si>
+    <t>avichaidevora.com/invitation/42652</t>
+  </si>
+  <si>
+    <t>other people</t>
+  </si>
+  <si>
+    <t>אנשים אחרים</t>
+  </si>
+  <si>
+    <t>viruses.live@gmail.com</t>
+  </si>
+  <si>
+    <t>1936</t>
+  </si>
+  <si>
+    <t>family 2</t>
+  </si>
+  <si>
+    <t>the Blanesses</t>
+  </si>
+  <si>
+    <t>משפחת בלה</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>avichaidevora.com/invitation/1936</t>
+  </si>
+  <si>
     <t>60107</t>
   </si>
   <si>
@@ -67,15 +133,6 @@
     <t>טסטינג פרסון 1</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>2015-04-23 10:11</t>
-  </si>
-  <si>
-    <t>Vegan</t>
-  </si>
-  <si>
     <t>Groom</t>
   </si>
   <si>
@@ -94,40 +151,22 @@
     <t>טסטינג פרסון 2</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>GlutenFree</t>
-  </si>
-  <si>
     <t>2@2.com</t>
   </si>
   <si>
-    <t>42652</t>
-  </si>
-  <si>
-    <t>family</t>
-  </si>
-  <si>
-    <t>the Moskovitzes</t>
-  </si>
-  <si>
-    <t>משפחת מוסקוביץ</t>
-  </si>
-  <si>
-    <t>2015-04-23 12:45</t>
-  </si>
-  <si>
-    <t>Bride</t>
-  </si>
-  <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>reyley1014@gmail.com</t>
-  </si>
-  <si>
-    <t>avichaidevora.com/invitation/42652</t>
+    <t>88850</t>
+  </si>
+  <si>
+    <t>sththrtger</t>
+  </si>
+  <si>
+    <t>srhsth</t>
+  </si>
+  <si>
+    <t>httshtrh</t>
+  </si>
+  <si>
+    <t>avichaidevora.com/invitation/88850</t>
   </si>
   <si>
     <t>20349</t>
@@ -142,7 +181,7 @@
     <t>חבר מהצבא</t>
   </si>
   <si>
-    <t>2015-04-23 12:43</t>
+    <t>Hebrew</t>
   </si>
   <si>
     <t>Army</t>
@@ -155,33 +194,6 @@
   </si>
   <si>
     <t>אורח/ת</t>
-  </si>
-  <si>
-    <t>Vegetarian</t>
-  </si>
-  <si>
-    <t>88850</t>
-  </si>
-  <si>
-    <t>sththrtger</t>
-  </si>
-  <si>
-    <t>srhsth</t>
-  </si>
-  <si>
-    <t>httshtrh</t>
-  </si>
-  <si>
-    <t>Maybe</t>
-  </si>
-  <si>
-    <t>2015-04-21 16:57</t>
-  </si>
-  <si>
-    <t>Both</t>
-  </si>
-  <si>
-    <t>avichaidevora.com/invitation/88850</t>
   </si>
 </sst>
 </file>
@@ -538,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -551,7 +563,7 @@
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
@@ -563,7 +575,7 @@
     <col min="17" max="17" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,38 +615,39 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G2" s="2">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
@@ -644,202 +657,296 @@
       <c r="M2" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N2" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>23</v>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2">
-        <v>5</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="2" t="s">
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2" t="s">
-        <v>44</v>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="2" t="s">
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="2">
+      <c r="C8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H8" s="2">
         <v>0</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2" t="s">
+      <c r="I8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>55</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>